<commit_message>
Update Rummi-BAC-11-Catálogo de atributos y relaciones.xlsx
</commit_message>
<xml_diff>
--- a/HT-2/Rummi-BAC-11-Catálogo de atributos y relaciones.xlsx
+++ b/HT-2/Rummi-BAC-11-Catálogo de atributos y relaciones.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ca42e1a7130a379e/Uniandes/Quinto Semestre/Arqui Emp/Hojas de trabajo/^N2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chech\Documents\GitHub\p3\arquiemp\HT-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="13_ncr:1_{29177F52-E3D4-43EB-9CF1-7EC259C5E081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E67BDD21-5E11-4BC5-A9DF-DFBEB033A755}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41ADDD0-D9D4-4DCB-B4D4-A2C292004F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
   </bookViews>
@@ -350,15 +350,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -369,12 +375,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -694,7 +694,7 @@
   <dimension ref="B2:D44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -741,7 +741,7 @@
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="24" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -749,24 +749,24 @@
       </c>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="23"/>
+    <row r="8" spans="2:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="26"/>
       <c r="C8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="10" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="23"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="9"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="23"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="10" t="s">
         <v>7</v>
       </c>
@@ -775,7 +775,7 @@
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="24"/>
+      <c r="B11" s="25"/>
       <c r="C11" s="11" t="s">
         <v>12</v>
       </c>
@@ -784,7 +784,7 @@
       </c>
     </row>
     <row r="12" spans="2:4" ht="28" x14ac:dyDescent="0.3">
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="24" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="18" t="s">
@@ -795,16 +795,16 @@
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" s="24"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="17" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="27" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="18" t="s">
@@ -813,14 +813,14 @@
       <c r="D14" s="16"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="26"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="18" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="16"/>
     </row>
     <row r="16" spans="2:4" ht="42" x14ac:dyDescent="0.3">
-      <c r="B16" s="27"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10" t="s">
         <v>23</v>
       </c>
@@ -829,7 +829,7 @@
       </c>
     </row>
     <row r="17" spans="2:4" ht="28" x14ac:dyDescent="0.3">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -840,7 +840,7 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="28" x14ac:dyDescent="0.3">
-      <c r="B18" s="28"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="10" t="s">
         <v>26</v>
       </c>
@@ -849,7 +849,7 @@
       </c>
     </row>
     <row r="19" spans="2:4" ht="28" x14ac:dyDescent="0.3">
-      <c r="B19" s="28"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="10" t="s">
         <v>29</v>
       </c>
@@ -858,14 +858,14 @@
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="30"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="16"/>
     </row>
     <row r="21" spans="2:4" ht="28" x14ac:dyDescent="0.3">
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="10" t="s">
@@ -876,7 +876,7 @@
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="28"/>
+      <c r="B22" s="30"/>
       <c r="C22" s="10" t="s">
         <v>32</v>
       </c>
@@ -885,7 +885,7 @@
       </c>
     </row>
     <row r="23" spans="2:4" ht="28" x14ac:dyDescent="0.3">
-      <c r="B23" s="28"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="14" t="s">
         <v>34</v>
       </c>
@@ -894,14 +894,14 @@
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B24" s="30"/>
+      <c r="B24" s="23"/>
       <c r="C24" s="14" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="16"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="12" t="s">
@@ -912,7 +912,7 @@
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B26" s="26"/>
+      <c r="B26" s="28"/>
       <c r="C26" s="13" t="s">
         <v>47</v>
       </c>
@@ -921,7 +921,7 @@
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B27" s="26"/>
+      <c r="B27" s="28"/>
       <c r="C27" s="10" t="s">
         <v>16</v>
       </c>
@@ -930,7 +930,7 @@
       </c>
     </row>
     <row r="28" spans="2:4" ht="28" x14ac:dyDescent="0.3">
-      <c r="B28" s="27"/>
+      <c r="B28" s="29"/>
       <c r="C28" s="10" t="s">
         <v>17</v>
       </c>
@@ -939,7 +939,7 @@
       </c>
     </row>
     <row r="29" spans="2:4" ht="28" x14ac:dyDescent="0.3">
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="22" t="s">
         <v>44</v>
       </c>
       <c r="C29" s="10" t="s">
@@ -950,7 +950,7 @@
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B30" s="30"/>
+      <c r="B30" s="23"/>
       <c r="C30" s="13" t="s">
         <v>14</v>
       </c>
@@ -959,7 +959,7 @@
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="24" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="10" t="s">
@@ -970,7 +970,7 @@
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B32" s="24"/>
+      <c r="B32" s="25"/>
       <c r="C32" s="9" t="s">
         <v>38</v>
       </c>

</xml_diff>